<commit_message>
Added APK and comments to the code
</commit_message>
<xml_diff>
--- a/Zeitplanen.xlsx
+++ b/Zeitplanen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elias\Documents\GitHub\Project 335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC74762-FD25-4914-9036-97133F5242C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD29D257-1D0C-4599-B335-13D28FCA686E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{4B305CFC-C0B3-4155-8BAF-9941DD21C0F0}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Planen</t>
   </si>
@@ -112,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +135,18 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="5" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
@@ -165,21 +177,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,16 +509,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D4B60CB-9A91-4A55-BDDC-A9937FEA8F07}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="15" width="5.453125" customWidth="1"/>
+    <col min="2" max="11" width="5.453125" customWidth="1"/>
+    <col min="12" max="15" width="5.453125" style="10" customWidth="1"/>
     <col min="16" max="16" width="4.7265625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.26953125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="4.7265625" bestFit="1" customWidth="1"/>
@@ -518,34 +534,30 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="5">
+      <c r="B1" s="7">
         <v>44963</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7">
         <v>44964</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7">
         <v>44965</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7">
         <v>44966</v>
       </c>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5">
+      <c r="I1" s="7"/>
+      <c r="J1" s="7">
         <v>44967</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5">
-        <v>44968</v>
-      </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5">
-        <v>44969</v>
-      </c>
-      <c r="O1" s="5"/>
+      <c r="K1" s="7"/>
+      <c r="L1"/>
+      <c r="M1"/>
+      <c r="N1"/>
+      <c r="O1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -579,94 +591,86 @@
       <c r="K2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
     </row>
     <row r="4" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
     </row>
     <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
     </row>
     <row r="6" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
@@ -676,54 +680,54 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
     </row>
     <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+    </row>
+    <row r="9" spans="1:15" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
@@ -737,10 +741,10 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
@@ -754,10 +758,10 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
@@ -771,10 +775,10 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
@@ -788,10 +792,10 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
@@ -805,10 +809,10 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
@@ -822,10 +826,10 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="3"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
@@ -839,10 +843,10 @@
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
@@ -856,10 +860,10 @@
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
-      <c r="O17" s="3"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="2"/>
@@ -873,16 +877,26 @@
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="L1:M1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="F1:G1"/>

</xml_diff>